<commit_message>
feat: added SB26 test dataset
</commit_message>
<xml_diff>
--- a/testdata/SB26/amp_batches.xlsx
+++ b/testdata/SB26/amp_batches.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10514"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10611"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/fdb589/Desktop/SB26-subset/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/fdb589/Share/dangpu01fl/projects/proks_et_al_2022/pipeline/SB26/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9733EFBE-B886-3B43-B94D-75C0140752DA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4257B315-3971-6C47-A8D5-E33D5D59B992}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3740" yWindow="1700" windowWidth="23260" windowHeight="13180" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="57">
   <si>
     <t>Amp_batch_ID</t>
   </si>
@@ -60,22 +60,145 @@
     <t>TGAT</t>
   </si>
   <si>
+    <t>Mars_1</t>
+  </si>
+  <si>
     <t>AB339</t>
   </si>
   <si>
+    <t>AB340</t>
+  </si>
+  <si>
+    <t>AB341</t>
+  </si>
+  <si>
+    <t>AB342</t>
+  </si>
+  <si>
+    <t>AB343</t>
+  </si>
+  <si>
+    <t>AB344</t>
+  </si>
+  <si>
+    <t>AB345</t>
+  </si>
+  <si>
+    <t>AB346</t>
+  </si>
+  <si>
+    <t>AB347</t>
+  </si>
+  <si>
+    <t>AB348</t>
+  </si>
+  <si>
+    <t>AB349</t>
+  </si>
+  <si>
+    <t>AB350</t>
+  </si>
+  <si>
+    <t>AB351</t>
+  </si>
+  <si>
+    <t>AB352</t>
+  </si>
+  <si>
     <t>SB26</t>
   </si>
   <si>
+    <t>TCTA</t>
+  </si>
+  <si>
+    <t>ACTT</t>
+  </si>
+  <si>
+    <t>CGCC</t>
+  </si>
+  <si>
+    <t>AAAC</t>
+  </si>
+  <si>
+    <t>GCGC</t>
+  </si>
+  <si>
+    <t>TTTC</t>
+  </si>
+  <si>
+    <t>GGTA</t>
+  </si>
+  <si>
+    <t>TCCG</t>
+  </si>
+  <si>
+    <t>AGGG</t>
+  </si>
+  <si>
+    <t>TAGA</t>
+  </si>
+  <si>
+    <t>CGGT</t>
+  </si>
+  <si>
+    <t>GCAT</t>
+  </si>
+  <si>
+    <t>GATC</t>
+  </si>
+  <si>
     <t>TECH_ES</t>
   </si>
   <si>
+    <t>TECH_MEF</t>
+  </si>
+  <si>
+    <t>TECH_MEF_ES</t>
+  </si>
+  <si>
     <t>Hadas</t>
   </si>
   <si>
     <t>ES#7_poolA</t>
   </si>
   <si>
-    <t>Mars_2</t>
+    <t>ES#7_poolH</t>
+  </si>
+  <si>
+    <t>ES #5_poolA</t>
+  </si>
+  <si>
+    <t>ES #5_poolH</t>
+  </si>
+  <si>
+    <t>MEF #12_poolA</t>
+  </si>
+  <si>
+    <t>MEF #12_poolH</t>
+  </si>
+  <si>
+    <t>ES/MEF #21_poolA</t>
+  </si>
+  <si>
+    <t>ES/MEF #21_poolH</t>
+  </si>
+  <si>
+    <t>ES/MEF #23_poolA</t>
+  </si>
+  <si>
+    <t>ES/MEF #23_poolH</t>
+  </si>
+  <si>
+    <t>MEF #13_poolA</t>
+  </si>
+  <si>
+    <t>MEF #13_poolH</t>
+  </si>
+  <si>
+    <t>ES/MEF #20_poolA</t>
+  </si>
+  <si>
+    <t>ES/MEF #20_poolH</t>
   </si>
 </sst>
 </file>
@@ -402,10 +525,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H2"/>
+  <dimension ref="A1:H15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="H19" sqref="H19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -448,13 +571,13 @@
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B2" t="s">
-        <v>11</v>
+        <v>25</v>
       </c>
       <c r="C2" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="D2" t="s">
         <v>9</v>
@@ -463,13 +586,351 @@
         <v>8</v>
       </c>
       <c r="F2" t="s">
+        <v>39</v>
+      </c>
+      <c r="G2" t="s">
+        <v>42</v>
+      </c>
+      <c r="H2" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
         <v>12</v>
       </c>
-      <c r="G2" t="s">
+      <c r="B3" t="s">
+        <v>25</v>
+      </c>
+      <c r="C3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D3" t="s">
+        <v>26</v>
+      </c>
+      <c r="E3" t="s">
+        <v>8</v>
+      </c>
+      <c r="F3" t="s">
+        <v>39</v>
+      </c>
+      <c r="G3" t="s">
+        <v>42</v>
+      </c>
+      <c r="H3" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
         <v>13</v>
       </c>
-      <c r="H2" t="s">
+      <c r="B4" t="s">
+        <v>25</v>
+      </c>
+      <c r="C4" t="s">
+        <v>10</v>
+      </c>
+      <c r="D4" t="s">
+        <v>27</v>
+      </c>
+      <c r="E4" t="s">
+        <v>8</v>
+      </c>
+      <c r="F4" t="s">
+        <v>39</v>
+      </c>
+      <c r="G4" t="s">
+        <v>42</v>
+      </c>
+      <c r="H4" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
         <v>14</v>
+      </c>
+      <c r="B5" t="s">
+        <v>25</v>
+      </c>
+      <c r="C5" t="s">
+        <v>10</v>
+      </c>
+      <c r="D5" t="s">
+        <v>28</v>
+      </c>
+      <c r="E5" t="s">
+        <v>8</v>
+      </c>
+      <c r="F5" t="s">
+        <v>39</v>
+      </c>
+      <c r="G5" t="s">
+        <v>42</v>
+      </c>
+      <c r="H5" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>15</v>
+      </c>
+      <c r="B6" t="s">
+        <v>25</v>
+      </c>
+      <c r="C6" t="s">
+        <v>10</v>
+      </c>
+      <c r="D6" t="s">
+        <v>29</v>
+      </c>
+      <c r="E6" t="s">
+        <v>8</v>
+      </c>
+      <c r="F6" t="s">
+        <v>40</v>
+      </c>
+      <c r="G6" t="s">
+        <v>42</v>
+      </c>
+      <c r="H6" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>16</v>
+      </c>
+      <c r="B7" t="s">
+        <v>25</v>
+      </c>
+      <c r="C7" t="s">
+        <v>10</v>
+      </c>
+      <c r="D7" t="s">
+        <v>30</v>
+      </c>
+      <c r="E7" t="s">
+        <v>8</v>
+      </c>
+      <c r="F7" t="s">
+        <v>40</v>
+      </c>
+      <c r="G7" t="s">
+        <v>42</v>
+      </c>
+      <c r="H7" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>17</v>
+      </c>
+      <c r="B8" t="s">
+        <v>25</v>
+      </c>
+      <c r="C8" t="s">
+        <v>10</v>
+      </c>
+      <c r="D8" t="s">
+        <v>31</v>
+      </c>
+      <c r="E8" t="s">
+        <v>8</v>
+      </c>
+      <c r="F8" t="s">
+        <v>41</v>
+      </c>
+      <c r="G8" t="s">
+        <v>42</v>
+      </c>
+      <c r="H8" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>18</v>
+      </c>
+      <c r="B9" t="s">
+        <v>25</v>
+      </c>
+      <c r="C9" t="s">
+        <v>10</v>
+      </c>
+      <c r="D9" t="s">
+        <v>32</v>
+      </c>
+      <c r="E9" t="s">
+        <v>8</v>
+      </c>
+      <c r="F9" t="s">
+        <v>41</v>
+      </c>
+      <c r="G9" t="s">
+        <v>42</v>
+      </c>
+      <c r="H9" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>19</v>
+      </c>
+      <c r="B10" t="s">
+        <v>25</v>
+      </c>
+      <c r="C10" t="s">
+        <v>10</v>
+      </c>
+      <c r="D10" t="s">
+        <v>33</v>
+      </c>
+      <c r="E10" t="s">
+        <v>8</v>
+      </c>
+      <c r="F10" t="s">
+        <v>41</v>
+      </c>
+      <c r="G10" t="s">
+        <v>42</v>
+      </c>
+      <c r="H10" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>20</v>
+      </c>
+      <c r="B11" t="s">
+        <v>25</v>
+      </c>
+      <c r="C11" t="s">
+        <v>10</v>
+      </c>
+      <c r="D11" t="s">
+        <v>34</v>
+      </c>
+      <c r="E11" t="s">
+        <v>8</v>
+      </c>
+      <c r="F11" t="s">
+        <v>41</v>
+      </c>
+      <c r="G11" t="s">
+        <v>42</v>
+      </c>
+      <c r="H11" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>21</v>
+      </c>
+      <c r="B12" t="s">
+        <v>25</v>
+      </c>
+      <c r="C12" t="s">
+        <v>10</v>
+      </c>
+      <c r="D12" t="s">
+        <v>35</v>
+      </c>
+      <c r="E12" t="s">
+        <v>8</v>
+      </c>
+      <c r="F12" t="s">
+        <v>40</v>
+      </c>
+      <c r="G12" t="s">
+        <v>42</v>
+      </c>
+      <c r="H12" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>22</v>
+      </c>
+      <c r="B13" t="s">
+        <v>25</v>
+      </c>
+      <c r="C13" t="s">
+        <v>10</v>
+      </c>
+      <c r="D13" t="s">
+        <v>36</v>
+      </c>
+      <c r="E13" t="s">
+        <v>8</v>
+      </c>
+      <c r="F13" t="s">
+        <v>40</v>
+      </c>
+      <c r="G13" t="s">
+        <v>42</v>
+      </c>
+      <c r="H13" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>23</v>
+      </c>
+      <c r="B14" t="s">
+        <v>25</v>
+      </c>
+      <c r="C14" t="s">
+        <v>10</v>
+      </c>
+      <c r="D14" t="s">
+        <v>37</v>
+      </c>
+      <c r="E14" t="s">
+        <v>8</v>
+      </c>
+      <c r="F14" t="s">
+        <v>41</v>
+      </c>
+      <c r="G14" t="s">
+        <v>42</v>
+      </c>
+      <c r="H14" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>24</v>
+      </c>
+      <c r="B15" t="s">
+        <v>25</v>
+      </c>
+      <c r="C15" t="s">
+        <v>10</v>
+      </c>
+      <c r="D15" t="s">
+        <v>38</v>
+      </c>
+      <c r="E15" t="s">
+        <v>8</v>
+      </c>
+      <c r="F15" t="s">
+        <v>41</v>
+      </c>
+      <c r="G15" t="s">
+        <v>42</v>
+      </c>
+      <c r="H15" t="s">
+        <v>56</v>
       </c>
     </row>
   </sheetData>

</xml_diff>